<commit_message>
update ms learn urls
</commit_message>
<xml_diff>
--- a/Assessments/Exam-Msft-AI-100-Self-Assessment-Build5Nines.xlsx
+++ b/Assessments/Exam-Msft-AI-100-Self-Assessment-Build5Nines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\exam-assessments\Assessments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="251" documentId="13_ncr:1_{A929D29F-BE51-4577-84D6-EA058C0D9C8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DE8DDE42-447D-4466-8D2E-70B5A20BE3A3}"/>
+  <xr:revisionPtr revIDLastSave="254" documentId="13_ncr:1_{A929D29F-BE51-4577-84D6-EA058C0D9C8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{01DAE8CC-AB3C-4836-A0A1-5578BBF75B52}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assessment Overview" sheetId="3" r:id="rId1"/>
@@ -128,7 +128,7 @@
     <t>Keep in mind that all exam Objective Domain info/text is copyright by Microsoft.</t>
   </si>
   <si>
-    <t>Self Assessment last updated November 13, 2019</t>
+    <t>Self Assessment last updated November 18, 2019</t>
   </si>
   <si>
     <t>Objective Domain</t>
@@ -537,10 +537,10 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1665,7 +1665,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>

</xml_diff>